<commit_message>
chats atualizado + notificacao
</commit_message>
<xml_diff>
--- a/views/compras/relatorios/relatorio_categorias_2025.xlsx
+++ b/views/compras/relatorios/relatorio_categorias_2025.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="44">
   <si>
     <t>RELATORIO RESUMO GERAL CLINICA PARQUE - 2025</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>AQUISICAO</t>
+  </si>
+  <si>
+    <t>EQUIPAMENTOS</t>
   </si>
   <si>
     <t>LENTE DE CONTATO</t>
@@ -577,10 +580,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:P64"/>
+  <dimension ref="A1:P65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="B64" sqref="B64"/>
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -593,7 +596,7 @@
     <col min="6" max="6" width="17.567" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="17.567" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="17.567" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="10.426" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="17.567" bestFit="true" customWidth="true" style="0"/>
     <col min="10" max="10" width="12.854" bestFit="true" customWidth="true" style="0"/>
     <col min="11" max="11" width="11.569" bestFit="true" customWidth="true" style="0"/>
     <col min="12" max="12" width="12.854" bestFit="true" customWidth="true" style="0"/>
@@ -691,26 +694,14 @@
       <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="6">
-        <v>11883.89</v>
-      </c>
-      <c r="C4" s="6">
-        <v>15065.67</v>
-      </c>
-      <c r="D4" s="6">
-        <v>15631.76</v>
-      </c>
-      <c r="E4" s="6">
-        <v>5724.9</v>
-      </c>
-      <c r="F4" s="6">
-        <v>7252.68</v>
-      </c>
-      <c r="G4" s="6">
-        <v>13471.12</v>
-      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
       <c r="H4" s="6">
-        <v>2506.59</v>
+        <v>34000.0</v>
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
@@ -718,7 +709,7 @@
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
       <c r="N4" s="8">
-        <v>71536.61</v>
+        <v>34000.0</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -726,85 +717,93 @@
         <v>17</v>
       </c>
       <c r="B5" s="6">
-        <v>3896.76</v>
+        <v>11883.89</v>
       </c>
       <c r="C5" s="6">
-        <v>30792.26</v>
+        <v>15065.67</v>
       </c>
       <c r="D5" s="6">
-        <v>250.0</v>
+        <v>15631.76</v>
       </c>
       <c r="E5" s="6">
-        <v>30944.76</v>
+        <v>5724.9</v>
       </c>
       <c r="F5" s="6">
-        <v>676.0</v>
+        <v>7252.68</v>
       </c>
       <c r="G5" s="6">
-        <v>23554.17</v>
+        <v>13471.12</v>
       </c>
       <c r="H5" s="6">
-        <v>2947.0</v>
-      </c>
-      <c r="I5" s="6"/>
+        <v>11329.93</v>
+      </c>
+      <c r="I5" s="6">
+        <v>1768.97</v>
+      </c>
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
       <c r="M5" s="6"/>
       <c r="N5" s="8">
-        <v>93060.95</v>
+        <v>82128.92</v>
       </c>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
+      <c r="B6" s="6">
+        <v>3896.76</v>
+      </c>
+      <c r="C6" s="6">
+        <v>30792.26</v>
+      </c>
       <c r="D6" s="6">
-        <v>270.0</v>
+        <v>250.0</v>
       </c>
       <c r="E6" s="6">
-        <v>1482.0</v>
+        <v>30944.76</v>
       </c>
       <c r="F6" s="6">
-        <v>1878.95</v>
+        <v>676.0</v>
       </c>
       <c r="G6" s="6">
-        <v>108.35</v>
+        <v>23554.17</v>
       </c>
       <c r="H6" s="6">
-        <v>1575.0</v>
-      </c>
-      <c r="I6" s="6"/>
+        <v>2947.0</v>
+      </c>
+      <c r="I6" s="6">
+        <v>735.0</v>
+      </c>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
       <c r="N6" s="8">
-        <v>5314.3</v>
+        <v>93795.95</v>
       </c>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="6">
-        <v>1188.0</v>
-      </c>
-      <c r="C7" s="6">
-        <v>210.0</v>
-      </c>
-      <c r="D7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6">
+        <v>270.0</v>
+      </c>
       <c r="E7" s="6">
-        <v>451.97</v>
-      </c>
-      <c r="F7" s="6"/>
+        <v>1482.0</v>
+      </c>
+      <c r="F7" s="6">
+        <v>1878.95</v>
+      </c>
       <c r="G7" s="6">
-        <v>274.16</v>
+        <v>108.35</v>
       </c>
       <c r="H7" s="6">
-        <v>439.99</v>
+        <v>1575.0</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
@@ -812,73 +811,73 @@
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
       <c r="N7" s="8">
-        <v>2564.12</v>
+        <v>5314.3</v>
       </c>
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="6"/>
+      <c r="B8" s="6">
+        <v>1188.0</v>
+      </c>
       <c r="C8" s="6">
-        <v>3981.6</v>
-      </c>
-      <c r="D8" s="6">
-        <v>1550.4</v>
-      </c>
+        <v>210.0</v>
+      </c>
+      <c r="D8" s="6"/>
       <c r="E8" s="6">
-        <v>1837.16</v>
-      </c>
-      <c r="F8" s="6">
-        <v>1614.39</v>
-      </c>
+        <v>451.97</v>
+      </c>
+      <c r="F8" s="6"/>
       <c r="G8" s="6">
-        <v>212.66</v>
+        <v>274.16</v>
       </c>
       <c r="H8" s="6">
-        <v>1375.79</v>
-      </c>
-      <c r="I8" s="6"/>
+        <v>502.39</v>
+      </c>
+      <c r="I8" s="6">
+        <v>447.9</v>
+      </c>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
       <c r="N8" s="8">
-        <v>10572.0</v>
+        <v>3074.42</v>
       </c>
     </row>
     <row r="9" spans="1:16">
       <c r="A9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="6">
-        <v>2169.8</v>
-      </c>
+      <c r="B9" s="6"/>
       <c r="C9" s="6">
-        <v>10504.54</v>
+        <v>3981.6</v>
       </c>
       <c r="D9" s="6">
-        <v>9256.77</v>
+        <v>1550.4</v>
       </c>
       <c r="E9" s="6">
-        <v>6704.75</v>
+        <v>1837.16</v>
       </c>
       <c r="F9" s="6">
-        <v>8011.43</v>
+        <v>1614.39</v>
       </c>
       <c r="G9" s="6">
-        <v>8266.9</v>
+        <v>212.66</v>
       </c>
       <c r="H9" s="6">
-        <v>5949.48</v>
-      </c>
-      <c r="I9" s="6"/>
+        <v>1423.19</v>
+      </c>
+      <c r="I9" s="6">
+        <v>1264.0</v>
+      </c>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
       <c r="N9" s="8">
-        <v>50863.67</v>
+        <v>11883.4</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -886,55 +885,71 @@
         <v>22</v>
       </c>
       <c r="B10" s="6">
-        <v>385.33</v>
+        <v>2169.8</v>
       </c>
       <c r="C10" s="6">
-        <v>450.4</v>
+        <v>10504.54</v>
       </c>
       <c r="D10" s="6">
-        <v>794.42</v>
+        <v>9256.77</v>
       </c>
       <c r="E10" s="6">
-        <v>1762.25</v>
+        <v>6704.75</v>
       </c>
       <c r="F10" s="6">
-        <v>1268.43</v>
+        <v>8011.43</v>
       </c>
       <c r="G10" s="6">
-        <v>965.11</v>
+        <v>8266.9</v>
       </c>
       <c r="H10" s="6">
-        <v>174.3</v>
-      </c>
-      <c r="I10" s="6"/>
+        <v>5949.48</v>
+      </c>
+      <c r="I10" s="6">
+        <v>5436.73</v>
+      </c>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
       <c r="M10" s="6"/>
       <c r="N10" s="8">
-        <v>5800.24</v>
+        <v>56300.4</v>
       </c>
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
+      <c r="B11" s="6">
+        <v>385.33</v>
+      </c>
+      <c r="C11" s="6">
+        <v>450.4</v>
+      </c>
+      <c r="D11" s="6">
+        <v>794.42</v>
+      </c>
+      <c r="E11" s="6">
+        <v>1762.25</v>
+      </c>
+      <c r="F11" s="6">
+        <v>1268.43</v>
+      </c>
+      <c r="G11" s="6">
+        <v>965.11</v>
+      </c>
       <c r="H11" s="6">
-        <v>2500.0</v>
-      </c>
-      <c r="I11" s="6"/>
+        <v>850.3</v>
+      </c>
+      <c r="I11" s="6">
+        <v>470.16</v>
+      </c>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
       <c r="M11" s="6"/>
       <c r="N11" s="8">
-        <v>2500.0</v>
+        <v>6946.4</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -942,55 +957,43 @@
         <v>24</v>
       </c>
       <c r="B12" s="6"/>
-      <c r="C12" s="6">
-        <v>97.47</v>
-      </c>
+      <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
+      <c r="H12" s="6">
+        <v>2500.0</v>
+      </c>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
       <c r="N12" s="8">
+        <v>2500.0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6">
         <v>97.47</v>
       </c>
-    </row>
-    <row r="13" spans="1:16">
-      <c r="A13" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="7">
-        <v>19523.78</v>
-      </c>
-      <c r="C13" s="7">
-        <v>61101.94</v>
-      </c>
-      <c r="D13" s="7">
-        <v>27753.35</v>
-      </c>
-      <c r="E13" s="7">
-        <v>48907.79</v>
-      </c>
-      <c r="F13" s="7">
-        <v>20701.88</v>
-      </c>
-      <c r="G13" s="7">
-        <v>47571.47</v>
-      </c>
-      <c r="H13" s="7">
-        <v>17468.15</v>
-      </c>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="9">
-        <v>243028.36</v>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="8">
+        <v>97.47</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -998,190 +1001,206 @@
         <v>26</v>
       </c>
       <c r="B14" s="7">
-        <f>IFERROR(AVERAGE(B3:B12),"")</f>
+        <v>19523.78</v>
+      </c>
+      <c r="C14" s="7">
+        <v>61101.94</v>
+      </c>
+      <c r="D14" s="7">
+        <v>27753.35</v>
+      </c>
+      <c r="E14" s="7">
+        <v>48907.79</v>
+      </c>
+      <c r="F14" s="7">
+        <v>20701.88</v>
+      </c>
+      <c r="G14" s="7">
+        <v>47571.47</v>
+      </c>
+      <c r="H14" s="7">
+        <v>61077.29</v>
+      </c>
+      <c r="I14" s="7">
+        <v>10122.76</v>
+      </c>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="9">
+        <v>296760.26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="7">
+        <f>IFERROR(AVERAGE(B3:B13),"")</f>
         <v>3904.756</v>
       </c>
-      <c r="C14" s="7">
-        <f>IFERROR(AVERAGE(C3:C12),"")</f>
+      <c r="C15" s="7">
+        <f>IFERROR(AVERAGE(C3:C13),"")</f>
         <v>8728.8485714286</v>
       </c>
-      <c r="D14" s="7">
-        <f>IFERROR(AVERAGE(D3:D12),"")</f>
+      <c r="D15" s="7">
+        <f>IFERROR(AVERAGE(D3:D13),"")</f>
         <v>4625.5583333333</v>
       </c>
-      <c r="E14" s="7">
-        <f>IFERROR(AVERAGE(E3:E12),"")</f>
+      <c r="E15" s="7">
+        <f>IFERROR(AVERAGE(E3:E13),"")</f>
         <v>6986.8271428571</v>
       </c>
-      <c r="F14" s="7">
-        <f>IFERROR(AVERAGE(F3:F12),"")</f>
+      <c r="F15" s="7">
+        <f>IFERROR(AVERAGE(F3:F13),"")</f>
         <v>3450.3133333333</v>
       </c>
-      <c r="G14" s="7">
-        <f>IFERROR(AVERAGE(G3:G12),"")</f>
+      <c r="G15" s="7">
+        <f>IFERROR(AVERAGE(G3:G13),"")</f>
         <v>5946.43375</v>
       </c>
-      <c r="H14" s="7">
-        <f>IFERROR(AVERAGE(H3:H12),"")</f>
-        <v>2183.51875</v>
-      </c>
-      <c r="I14" s="7" t="str">
-        <f>IFERROR(AVERAGE(I3:I12),"")</f>
+      <c r="H15" s="7">
+        <f>IFERROR(AVERAGE(H3:H13),"")</f>
+        <v>6786.3655555556</v>
+      </c>
+      <c r="I15" s="7">
+        <f>IFERROR(AVERAGE(I3:I13),"")</f>
+        <v>1687.1266666667</v>
+      </c>
+      <c r="J15" s="7" t="str">
+        <f>IFERROR(AVERAGE(J3:J13),"")</f>
         <v/>
       </c>
-      <c r="J14" s="7" t="str">
-        <f>IFERROR(AVERAGE(J3:J12),"")</f>
+      <c r="K15" s="7" t="str">
+        <f>IFERROR(AVERAGE(K3:K13),"")</f>
         <v/>
       </c>
-      <c r="K14" s="7" t="str">
-        <f>IFERROR(AVERAGE(K3:K12),"")</f>
+      <c r="L15" s="7" t="str">
+        <f>IFERROR(AVERAGE(L3:L13),"")</f>
         <v/>
       </c>
-      <c r="L14" s="7" t="str">
-        <f>IFERROR(AVERAGE(L3:L12),"")</f>
+      <c r="M15" s="7" t="str">
+        <f>IFERROR(AVERAGE(M3:M13),"")</f>
         <v/>
       </c>
-      <c r="M14" s="7" t="str">
-        <f>IFERROR(AVERAGE(M3:M12),"")</f>
-        <v/>
-      </c>
-      <c r="N14" s="9">
-        <f>IFERROR(AVERAGE(N3:N12),"")</f>
-        <v>24302.836</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16">
-      <c r="A16" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
+      <c r="N15" s="9">
+        <f>IFERROR(AVERAGE(N3:N13),"")</f>
+        <v>26978.205454545</v>
+      </c>
     </row>
     <row r="17" spans="1:16">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="A18" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B18" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G18" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="H18" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I17" s="3" t="s">
+      <c r="I18" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J17" s="3" t="s">
+      <c r="J18" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K17" s="3" t="s">
+      <c r="K18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L17" s="3" t="s">
+      <c r="L18" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="M17" s="3" t="s">
+      <c r="M18" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N17" s="3" t="s">
+      <c r="N18" s="3" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16">
-      <c r="A18" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="6">
-        <v>3302.47</v>
-      </c>
-      <c r="C18" s="6">
-        <v>5362.34</v>
-      </c>
-      <c r="D18" s="6">
-        <v>4270.05</v>
-      </c>
-      <c r="E18" s="6">
-        <v>5257.15</v>
-      </c>
-      <c r="F18" s="6">
-        <v>6803.29</v>
-      </c>
-      <c r="G18" s="6">
-        <v>3222.73</v>
-      </c>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="8">
-        <v>28218.03</v>
       </c>
     </row>
     <row r="19" spans="1:16">
       <c r="A19" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="6">
-        <v>870.0</v>
-      </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
+        <v>3302.47</v>
+      </c>
+      <c r="C19" s="6">
+        <v>5362.34</v>
+      </c>
+      <c r="D19" s="6">
+        <v>4270.05</v>
+      </c>
       <c r="E19" s="6">
-        <v>273.0</v>
-      </c>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
+        <v>5257.15</v>
+      </c>
+      <c r="F19" s="6">
+        <v>6803.29</v>
+      </c>
+      <c r="G19" s="6">
+        <v>3569.62</v>
+      </c>
+      <c r="H19" s="6">
+        <v>6003.95</v>
+      </c>
+      <c r="I19" s="6">
+        <v>5258.21</v>
+      </c>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
       <c r="N19" s="8">
-        <v>1143.0</v>
+        <v>39827.08</v>
       </c>
     </row>
     <row r="20" spans="1:16">
       <c r="A20" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6">
-        <v>210.0</v>
-      </c>
+      <c r="B20" s="6">
+        <v>870.0</v>
+      </c>
+      <c r="C20" s="6"/>
       <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
+      <c r="E20" s="6">
+        <v>273.0</v>
+      </c>
       <c r="F20" s="6"/>
-      <c r="G20" s="6">
-        <v>68.24</v>
-      </c>
+      <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
@@ -1189,7 +1208,7 @@
       <c r="L20" s="6"/>
       <c r="M20" s="6"/>
       <c r="N20" s="8">
-        <v>278.24</v>
+        <v>1143.0</v>
       </c>
     </row>
     <row r="21" spans="1:16">
@@ -1197,21 +1216,25 @@
         <v>20</v>
       </c>
       <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
+      <c r="C21" s="6">
+        <v>210.0</v>
+      </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6">
-        <v>809.97</v>
-      </c>
-      <c r="I21" s="6"/>
+      <c r="G21" s="6">
+        <v>68.24</v>
+      </c>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6">
+        <v>410.0</v>
+      </c>
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
       <c r="M21" s="6"/>
       <c r="N21" s="8">
-        <v>809.97</v>
+        <v>688.24</v>
       </c>
     </row>
     <row r="22" spans="1:16">
@@ -1219,40 +1242,34 @@
         <v>21</v>
       </c>
       <c r="B22" s="6"/>
-      <c r="C22" s="6">
-        <v>2341.21</v>
-      </c>
+      <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
+      <c r="H22" s="6">
+        <v>809.97</v>
+      </c>
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
       <c r="N22" s="8">
-        <v>2341.21</v>
+        <v>809.97</v>
       </c>
     </row>
     <row r="23" spans="1:16">
       <c r="A23" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="6">
-        <v>723.5</v>
-      </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6">
-        <v>1147.77</v>
-      </c>
-      <c r="E23" s="6">
-        <v>161.15</v>
-      </c>
-      <c r="F23" s="6">
-        <v>965.41</v>
-      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6">
+        <v>2341.21</v>
+      </c>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
@@ -1261,41 +1278,37 @@
       <c r="L23" s="6"/>
       <c r="M23" s="6"/>
       <c r="N23" s="8">
-        <v>2997.83</v>
+        <v>2341.21</v>
       </c>
     </row>
     <row r="24" spans="1:16">
-      <c r="A24" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="7">
-        <v>4895.97</v>
-      </c>
-      <c r="C24" s="7">
-        <v>7913.55</v>
-      </c>
-      <c r="D24" s="7">
-        <v>5417.82</v>
-      </c>
-      <c r="E24" s="7">
-        <v>5691.3</v>
-      </c>
-      <c r="F24" s="7">
-        <v>7768.7</v>
-      </c>
-      <c r="G24" s="7">
-        <v>3290.97</v>
-      </c>
-      <c r="H24" s="7">
-        <v>809.97</v>
-      </c>
-      <c r="I24" s="7"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="9">
-        <v>35788.28</v>
+      <c r="A24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="6">
+        <v>723.5</v>
+      </c>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6">
+        <v>1147.77</v>
+      </c>
+      <c r="E24" s="6">
+        <v>161.15</v>
+      </c>
+      <c r="F24" s="6">
+        <v>965.41</v>
+      </c>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6">
+        <v>1050.06</v>
+      </c>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="8">
+        <v>4047.89</v>
       </c>
     </row>
     <row r="25" spans="1:16">
@@ -1303,214 +1316,222 @@
         <v>26</v>
       </c>
       <c r="B25" s="7">
-        <f>IFERROR(AVERAGE(B18:B23),"")</f>
+        <v>4895.97</v>
+      </c>
+      <c r="C25" s="7">
+        <v>7913.55</v>
+      </c>
+      <c r="D25" s="7">
+        <v>5417.82</v>
+      </c>
+      <c r="E25" s="7">
+        <v>5691.3</v>
+      </c>
+      <c r="F25" s="7">
+        <v>7768.7</v>
+      </c>
+      <c r="G25" s="7">
+        <v>3637.86</v>
+      </c>
+      <c r="H25" s="7">
+        <v>7863.98</v>
+      </c>
+      <c r="I25" s="7">
+        <v>5668.21</v>
+      </c>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="9">
+        <v>48857.39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="7">
+        <f>IFERROR(AVERAGE(B19:B24),"")</f>
         <v>1631.99</v>
       </c>
-      <c r="C25" s="7">
-        <f>IFERROR(AVERAGE(C18:C23),"")</f>
+      <c r="C26" s="7">
+        <f>IFERROR(AVERAGE(C19:C24),"")</f>
         <v>2637.85</v>
       </c>
-      <c r="D25" s="7">
-        <f>IFERROR(AVERAGE(D18:D23),"")</f>
+      <c r="D26" s="7">
+        <f>IFERROR(AVERAGE(D19:D24),"")</f>
         <v>2708.91</v>
       </c>
-      <c r="E25" s="7">
-        <f>IFERROR(AVERAGE(E18:E23),"")</f>
+      <c r="E26" s="7">
+        <f>IFERROR(AVERAGE(E19:E24),"")</f>
         <v>1897.1</v>
       </c>
-      <c r="F25" s="7">
-        <f>IFERROR(AVERAGE(F18:F23),"")</f>
+      <c r="F26" s="7">
+        <f>IFERROR(AVERAGE(F19:F24),"")</f>
         <v>3884.35</v>
       </c>
-      <c r="G25" s="7">
-        <f>IFERROR(AVERAGE(G18:G23),"")</f>
-        <v>1645.485</v>
-      </c>
-      <c r="H25" s="7">
-        <f>IFERROR(AVERAGE(H18:H23),"")</f>
-        <v>809.97</v>
-      </c>
-      <c r="I25" s="7" t="str">
-        <f>IFERROR(AVERAGE(I18:I23),"")</f>
+      <c r="G26" s="7">
+        <f>IFERROR(AVERAGE(G19:G24),"")</f>
+        <v>1818.93</v>
+      </c>
+      <c r="H26" s="7">
+        <f>IFERROR(AVERAGE(H19:H24),"")</f>
+        <v>2621.3266666667</v>
+      </c>
+      <c r="I26" s="7">
+        <f>IFERROR(AVERAGE(I19:I24),"")</f>
+        <v>2834.105</v>
+      </c>
+      <c r="J26" s="7" t="str">
+        <f>IFERROR(AVERAGE(J19:J24),"")</f>
         <v/>
       </c>
-      <c r="J25" s="7" t="str">
-        <f>IFERROR(AVERAGE(J18:J23),"")</f>
+      <c r="K26" s="7" t="str">
+        <f>IFERROR(AVERAGE(K19:K24),"")</f>
         <v/>
       </c>
-      <c r="K25" s="7" t="str">
-        <f>IFERROR(AVERAGE(K18:K23),"")</f>
+      <c r="L26" s="7" t="str">
+        <f>IFERROR(AVERAGE(L19:L24),"")</f>
         <v/>
       </c>
-      <c r="L25" s="7" t="str">
-        <f>IFERROR(AVERAGE(L18:L23),"")</f>
+      <c r="M26" s="7" t="str">
+        <f>IFERROR(AVERAGE(M19:M24),"")</f>
         <v/>
       </c>
-      <c r="M25" s="7" t="str">
-        <f>IFERROR(AVERAGE(M18:M23),"")</f>
-        <v/>
-      </c>
-      <c r="N25" s="9">
-        <f>IFERROR(AVERAGE(N18:N23),"")</f>
-        <v>5964.7133333333</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16">
-      <c r="A27" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-      <c r="M27" s="4"/>
-      <c r="N27" s="4"/>
+      <c r="N26" s="9">
+        <f>IFERROR(AVERAGE(N19:N24),"")</f>
+        <v>8142.8983333333</v>
+      </c>
     </row>
     <row r="28" spans="1:16">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B29" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C29" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D29" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="E29" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F29" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="G29" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H28" s="3" t="s">
+      <c r="H29" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I28" s="3" t="s">
+      <c r="I29" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J28" s="3" t="s">
+      <c r="J29" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K28" s="3" t="s">
+      <c r="K29" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L28" s="3" t="s">
+      <c r="L29" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="M28" s="3" t="s">
+      <c r="M29" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N28" s="3" t="s">
+      <c r="N29" s="3" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16">
-      <c r="A29" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6">
-        <v>28.72</v>
-      </c>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="6"/>
-      <c r="M29" s="6"/>
-      <c r="N29" s="8">
-        <v>28.72</v>
       </c>
     </row>
     <row r="30" spans="1:16">
       <c r="A30" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
-      <c r="D30" s="6">
-        <v>1487.76</v>
-      </c>
-      <c r="E30" s="6">
-        <v>932.02</v>
-      </c>
-      <c r="F30" s="6">
-        <v>669.25</v>
-      </c>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6">
-        <v>595.3</v>
-      </c>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6">
+        <v>28.72</v>
+      </c>
+      <c r="H30" s="6"/>
       <c r="I30" s="6"/>
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
       <c r="L30" s="6"/>
       <c r="M30" s="6"/>
       <c r="N30" s="8">
-        <v>3684.33</v>
+        <v>28.72</v>
       </c>
     </row>
     <row r="31" spans="1:16">
       <c r="A31" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B31" s="6"/>
-      <c r="C31" s="6">
-        <v>210.0</v>
-      </c>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6">
+        <v>1487.76</v>
+      </c>
+      <c r="E31" s="6">
+        <v>932.02</v>
+      </c>
       <c r="F31" s="6">
-        <v>843.7</v>
+        <v>669.25</v>
       </c>
       <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
+      <c r="H31" s="6">
+        <v>1170.14</v>
+      </c>
+      <c r="I31" s="6">
+        <v>362.0</v>
+      </c>
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
       <c r="L31" s="6"/>
       <c r="M31" s="6"/>
       <c r="N31" s="8">
-        <v>1053.7</v>
+        <v>4621.17</v>
       </c>
     </row>
     <row r="32" spans="1:16">
       <c r="A32" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B32" s="6">
-        <v>597.55</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B32" s="6"/>
       <c r="C32" s="6">
-        <v>513.23</v>
-      </c>
-      <c r="D32" s="6">
-        <v>299.45</v>
-      </c>
+        <v>210.0</v>
+      </c>
+      <c r="D32" s="6"/>
       <c r="E32" s="6"/>
       <c r="F32" s="6">
-        <v>760.7</v>
-      </c>
-      <c r="G32" s="6">
-        <v>278.63</v>
-      </c>
+        <v>843.7</v>
+      </c>
+      <c r="G32" s="6"/>
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
       <c r="J32" s="6"/>
@@ -1518,41 +1539,37 @@
       <c r="L32" s="6"/>
       <c r="M32" s="6"/>
       <c r="N32" s="8">
+        <v>1053.7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
+      <c r="A33" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B33" s="6">
+        <v>597.55</v>
+      </c>
+      <c r="C33" s="6">
+        <v>513.23</v>
+      </c>
+      <c r="D33" s="6">
+        <v>299.45</v>
+      </c>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6">
+        <v>760.7</v>
+      </c>
+      <c r="G33" s="6">
+        <v>278.63</v>
+      </c>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
+      <c r="M33" s="6"/>
+      <c r="N33" s="8">
         <v>2449.56</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16">
-      <c r="A33" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B33" s="7">
-        <v>597.55</v>
-      </c>
-      <c r="C33" s="7">
-        <v>723.23</v>
-      </c>
-      <c r="D33" s="7">
-        <v>1787.21</v>
-      </c>
-      <c r="E33" s="7">
-        <v>932.02</v>
-      </c>
-      <c r="F33" s="7">
-        <v>2273.65</v>
-      </c>
-      <c r="G33" s="7">
-        <v>307.35</v>
-      </c>
-      <c r="H33" s="7">
-        <v>595.3</v>
-      </c>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="7"/>
-      <c r="L33" s="7"/>
-      <c r="M33" s="7"/>
-      <c r="N33" s="9">
-        <v>7216.31</v>
       </c>
     </row>
     <row r="34" spans="1:16">
@@ -1560,174 +1577,190 @@
         <v>26</v>
       </c>
       <c r="B34" s="7">
-        <f>IFERROR(AVERAGE(B29:B32),"")</f>
         <v>597.55</v>
       </c>
       <c r="C34" s="7">
-        <f>IFERROR(AVERAGE(C29:C32),"")</f>
+        <v>723.23</v>
+      </c>
+      <c r="D34" s="7">
+        <v>1787.21</v>
+      </c>
+      <c r="E34" s="7">
+        <v>932.02</v>
+      </c>
+      <c r="F34" s="7">
+        <v>2273.65</v>
+      </c>
+      <c r="G34" s="7">
+        <v>307.35</v>
+      </c>
+      <c r="H34" s="7">
+        <v>1170.14</v>
+      </c>
+      <c r="I34" s="7">
+        <v>362.0</v>
+      </c>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="9">
+        <v>8153.15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
+      <c r="A35" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35" s="7">
+        <f>IFERROR(AVERAGE(B30:B33),"")</f>
+        <v>597.55</v>
+      </c>
+      <c r="C35" s="7">
+        <f>IFERROR(AVERAGE(C30:C33),"")</f>
         <v>361.615</v>
       </c>
-      <c r="D34" s="7">
-        <f>IFERROR(AVERAGE(D29:D32),"")</f>
+      <c r="D35" s="7">
+        <f>IFERROR(AVERAGE(D30:D33),"")</f>
         <v>893.605</v>
       </c>
-      <c r="E34" s="7">
-        <f>IFERROR(AVERAGE(E29:E32),"")</f>
+      <c r="E35" s="7">
+        <f>IFERROR(AVERAGE(E30:E33),"")</f>
         <v>932.02</v>
       </c>
-      <c r="F34" s="7">
-        <f>IFERROR(AVERAGE(F29:F32),"")</f>
+      <c r="F35" s="7">
+        <f>IFERROR(AVERAGE(F30:F33),"")</f>
         <v>757.88333333333</v>
       </c>
-      <c r="G34" s="7">
-        <f>IFERROR(AVERAGE(G29:G32),"")</f>
+      <c r="G35" s="7">
+        <f>IFERROR(AVERAGE(G30:G33),"")</f>
         <v>153.675</v>
       </c>
-      <c r="H34" s="7">
-        <f>IFERROR(AVERAGE(H29:H32),"")</f>
-        <v>595.3</v>
-      </c>
-      <c r="I34" s="7" t="str">
-        <f>IFERROR(AVERAGE(I29:I32),"")</f>
+      <c r="H35" s="7">
+        <f>IFERROR(AVERAGE(H30:H33),"")</f>
+        <v>1170.14</v>
+      </c>
+      <c r="I35" s="7">
+        <f>IFERROR(AVERAGE(I30:I33),"")</f>
+        <v>362</v>
+      </c>
+      <c r="J35" s="7" t="str">
+        <f>IFERROR(AVERAGE(J30:J33),"")</f>
         <v/>
       </c>
-      <c r="J34" s="7" t="str">
-        <f>IFERROR(AVERAGE(J29:J32),"")</f>
+      <c r="K35" s="7" t="str">
+        <f>IFERROR(AVERAGE(K30:K33),"")</f>
         <v/>
       </c>
-      <c r="K34" s="7" t="str">
-        <f>IFERROR(AVERAGE(K29:K32),"")</f>
+      <c r="L35" s="7" t="str">
+        <f>IFERROR(AVERAGE(L30:L33),"")</f>
         <v/>
       </c>
-      <c r="L34" s="7" t="str">
-        <f>IFERROR(AVERAGE(L29:L32),"")</f>
+      <c r="M35" s="7" t="str">
+        <f>IFERROR(AVERAGE(M30:M33),"")</f>
         <v/>
       </c>
-      <c r="M34" s="7" t="str">
-        <f>IFERROR(AVERAGE(M29:M32),"")</f>
-        <v/>
-      </c>
-      <c r="N34" s="9">
-        <f>IFERROR(AVERAGE(N29:N32),"")</f>
-        <v>1804.0775</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16">
-      <c r="A36" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="4"/>
-      <c r="N36" s="4"/>
+      <c r="N35" s="9">
+        <f>IFERROR(AVERAGE(N30:N33),"")</f>
+        <v>2038.2875</v>
+      </c>
     </row>
     <row r="37" spans="1:16">
-      <c r="A37" s="11" t="s">
+      <c r="A37" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4"/>
+    </row>
+    <row r="38" spans="1:16">
+      <c r="A38" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B37" s="11" t="s">
+      <c r="B38" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C38" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D37" s="11" t="s">
+      <c r="D38" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E37" s="11" t="s">
+      <c r="E38" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F37" s="11" t="s">
+      <c r="F38" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G37" s="11" t="s">
+      <c r="G38" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H37" s="11" t="s">
+      <c r="H38" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="I37" s="11" t="s">
+      <c r="I38" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="J37" s="11" t="s">
+      <c r="J38" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="K37" s="11" t="s">
+      <c r="K38" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="L37" s="11" t="s">
+      <c r="L38" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="M37" s="11" t="s">
+      <c r="M38" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="N37" s="11" t="s">
+      <c r="N38" s="11" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16">
-      <c r="A38" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B38" s="6">
-        <v>12480.45</v>
-      </c>
-      <c r="C38" s="6">
-        <v>23466.32</v>
-      </c>
-      <c r="D38" s="6">
-        <v>15893.0</v>
-      </c>
-      <c r="E38" s="6">
-        <v>7276.95</v>
-      </c>
-      <c r="F38" s="6">
-        <v>32037.68</v>
-      </c>
-      <c r="G38" s="6">
-        <v>9621.18</v>
-      </c>
-      <c r="H38" s="6">
-        <v>5174.69</v>
-      </c>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
-      <c r="K38" s="6"/>
-      <c r="L38" s="6"/>
-      <c r="M38" s="6"/>
-      <c r="N38" s="8">
-        <v>105950.27</v>
       </c>
     </row>
     <row r="39" spans="1:16">
       <c r="A39" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="6"/>
+      <c r="B39" s="6">
+        <v>12480.45</v>
+      </c>
       <c r="C39" s="6">
-        <v>3900.0</v>
-      </c>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
+        <v>23466.32</v>
+      </c>
+      <c r="D39" s="6">
+        <v>15893.0</v>
+      </c>
+      <c r="E39" s="6">
+        <v>7276.95</v>
+      </c>
+      <c r="F39" s="6">
+        <v>32037.68</v>
+      </c>
+      <c r="G39" s="6">
+        <v>9621.18</v>
+      </c>
+      <c r="H39" s="6">
+        <v>20855.18</v>
+      </c>
+      <c r="I39" s="6">
+        <v>668.71</v>
+      </c>
       <c r="J39" s="6"/>
       <c r="K39" s="6"/>
       <c r="L39" s="6"/>
       <c r="M39" s="6"/>
       <c r="N39" s="8">
-        <v>3900.0</v>
+        <v>122299.47</v>
       </c>
     </row>
     <row r="40" spans="1:16">
@@ -1736,15 +1769,11 @@
       </c>
       <c r="B40" s="6"/>
       <c r="C40" s="6">
-        <v>1104.0</v>
+        <v>3900.0</v>
       </c>
       <c r="D40" s="6"/>
-      <c r="E40" s="6">
-        <v>873.0</v>
-      </c>
-      <c r="F40" s="6">
-        <v>594.0</v>
-      </c>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
       <c r="G40" s="6"/>
       <c r="H40" s="6"/>
       <c r="I40" s="6"/>
@@ -1753,87 +1782,79 @@
       <c r="L40" s="6"/>
       <c r="M40" s="6"/>
       <c r="N40" s="8">
-        <v>2571.0</v>
+        <v>3900.0</v>
       </c>
     </row>
     <row r="41" spans="1:16">
       <c r="A41" s="4" t="s">
-        <v>16</v>
+        <v>33</v>
       </c>
       <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
+      <c r="C41" s="6">
+        <v>1104.0</v>
+      </c>
       <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
+      <c r="E41" s="6">
+        <v>873.0</v>
+      </c>
+      <c r="F41" s="6">
+        <v>594.0</v>
+      </c>
       <c r="G41" s="6"/>
-      <c r="H41" s="6">
-        <v>788.31</v>
-      </c>
+      <c r="H41" s="6"/>
       <c r="I41" s="6"/>
       <c r="J41" s="6"/>
       <c r="K41" s="6"/>
       <c r="L41" s="6"/>
       <c r="M41" s="6"/>
       <c r="N41" s="8">
-        <v>788.31</v>
+        <v>2571.0</v>
       </c>
     </row>
     <row r="42" spans="1:16">
       <c r="A42" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B42" s="6"/>
-      <c r="C42" s="6">
-        <v>210.0</v>
-      </c>
+      <c r="C42" s="6"/>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
-      <c r="G42" s="6">
-        <v>340.0</v>
-      </c>
-      <c r="H42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6">
+        <v>788.31</v>
+      </c>
       <c r="I42" s="6"/>
       <c r="J42" s="6"/>
       <c r="K42" s="6"/>
       <c r="L42" s="6"/>
       <c r="M42" s="6"/>
       <c r="N42" s="8">
+        <v>788.31</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16">
+      <c r="A43" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6">
+        <v>210.0</v>
+      </c>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6">
+        <v>340.0</v>
+      </c>
+      <c r="H43" s="6"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="6"/>
+      <c r="K43" s="6"/>
+      <c r="L43" s="6"/>
+      <c r="M43" s="6"/>
+      <c r="N43" s="8">
         <v>550.0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16">
-      <c r="A43" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B43" s="7">
-        <v>12480.45</v>
-      </c>
-      <c r="C43" s="7">
-        <v>28680.32</v>
-      </c>
-      <c r="D43" s="7">
-        <v>15893.0</v>
-      </c>
-      <c r="E43" s="7">
-        <v>8149.95</v>
-      </c>
-      <c r="F43" s="7">
-        <v>32631.68</v>
-      </c>
-      <c r="G43" s="7">
-        <v>9961.18</v>
-      </c>
-      <c r="H43" s="7">
-        <v>5963.0</v>
-      </c>
-      <c r="I43" s="7"/>
-      <c r="J43" s="7"/>
-      <c r="K43" s="7"/>
-      <c r="L43" s="7"/>
-      <c r="M43" s="7"/>
-      <c r="N43" s="9">
-        <v>113759.58</v>
       </c>
     </row>
     <row r="44" spans="1:16">
@@ -1841,189 +1862,207 @@
         <v>26</v>
       </c>
       <c r="B44" s="7">
-        <f>IFERROR(AVERAGE(B38:B42),"")</f>
         <v>12480.45</v>
       </c>
       <c r="C44" s="7">
-        <f>IFERROR(AVERAGE(C38:C42),"")</f>
+        <v>28680.32</v>
+      </c>
+      <c r="D44" s="7">
+        <v>15893.0</v>
+      </c>
+      <c r="E44" s="7">
+        <v>8149.95</v>
+      </c>
+      <c r="F44" s="7">
+        <v>32631.68</v>
+      </c>
+      <c r="G44" s="7">
+        <v>9961.18</v>
+      </c>
+      <c r="H44" s="7">
+        <v>21643.49</v>
+      </c>
+      <c r="I44" s="7">
+        <v>668.71</v>
+      </c>
+      <c r="J44" s="7"/>
+      <c r="K44" s="7"/>
+      <c r="L44" s="7"/>
+      <c r="M44" s="7"/>
+      <c r="N44" s="9">
+        <v>130108.78</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16">
+      <c r="A45" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B45" s="7">
+        <f>IFERROR(AVERAGE(B39:B43),"")</f>
+        <v>12480.45</v>
+      </c>
+      <c r="C45" s="7">
+        <f>IFERROR(AVERAGE(C39:C43),"")</f>
         <v>7170.08</v>
       </c>
-      <c r="D44" s="7">
-        <f>IFERROR(AVERAGE(D38:D42),"")</f>
+      <c r="D45" s="7">
+        <f>IFERROR(AVERAGE(D39:D43),"")</f>
         <v>15893</v>
       </c>
-      <c r="E44" s="7">
-        <f>IFERROR(AVERAGE(E38:E42),"")</f>
+      <c r="E45" s="7">
+        <f>IFERROR(AVERAGE(E39:E43),"")</f>
         <v>4074.975</v>
       </c>
-      <c r="F44" s="7">
-        <f>IFERROR(AVERAGE(F38:F42),"")</f>
+      <c r="F45" s="7">
+        <f>IFERROR(AVERAGE(F39:F43),"")</f>
         <v>16315.84</v>
       </c>
-      <c r="G44" s="7">
-        <f>IFERROR(AVERAGE(G38:G42),"")</f>
+      <c r="G45" s="7">
+        <f>IFERROR(AVERAGE(G39:G43),"")</f>
         <v>4980.59</v>
       </c>
-      <c r="H44" s="7">
-        <f>IFERROR(AVERAGE(H38:H42),"")</f>
-        <v>2981.5</v>
-      </c>
-      <c r="I44" s="7" t="str">
-        <f>IFERROR(AVERAGE(I38:I42),"")</f>
+      <c r="H45" s="7">
+        <f>IFERROR(AVERAGE(H39:H43),"")</f>
+        <v>10821.745</v>
+      </c>
+      <c r="I45" s="7">
+        <f>IFERROR(AVERAGE(I39:I43),"")</f>
+        <v>668.71</v>
+      </c>
+      <c r="J45" s="7" t="str">
+        <f>IFERROR(AVERAGE(J39:J43),"")</f>
         <v/>
       </c>
-      <c r="J44" s="7" t="str">
-        <f>IFERROR(AVERAGE(J38:J42),"")</f>
+      <c r="K45" s="7" t="str">
+        <f>IFERROR(AVERAGE(K39:K43),"")</f>
         <v/>
       </c>
-      <c r="K44" s="7" t="str">
-        <f>IFERROR(AVERAGE(K38:K42),"")</f>
+      <c r="L45" s="7" t="str">
+        <f>IFERROR(AVERAGE(L39:L43),"")</f>
         <v/>
       </c>
-      <c r="L44" s="7" t="str">
-        <f>IFERROR(AVERAGE(L38:L42),"")</f>
+      <c r="M45" s="7" t="str">
+        <f>IFERROR(AVERAGE(M39:M43),"")</f>
         <v/>
       </c>
-      <c r="M44" s="7" t="str">
-        <f>IFERROR(AVERAGE(M38:M42),"")</f>
-        <v/>
-      </c>
-      <c r="N44" s="9">
-        <f>IFERROR(AVERAGE(N38:N42),"")</f>
-        <v>22751.916</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16">
-      <c r="A46" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
-      <c r="H46" s="4"/>
-      <c r="I46" s="4"/>
-      <c r="J46" s="4"/>
-      <c r="K46" s="4"/>
-      <c r="L46" s="4"/>
-      <c r="M46" s="4"/>
-      <c r="N46" s="4"/>
+      <c r="N45" s="9">
+        <f>IFERROR(AVERAGE(N39:N43),"")</f>
+        <v>26021.756</v>
+      </c>
     </row>
     <row r="47" spans="1:16">
-      <c r="A47" s="11" t="s">
+      <c r="A47" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="4"/>
+      <c r="L47" s="4"/>
+      <c r="M47" s="4"/>
+      <c r="N47" s="4"/>
+    </row>
+    <row r="48" spans="1:16">
+      <c r="A48" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B47" s="11" t="s">
+      <c r="B48" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C47" s="11" t="s">
+      <c r="C48" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D47" s="11" t="s">
+      <c r="D48" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E47" s="11" t="s">
+      <c r="E48" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F47" s="11" t="s">
+      <c r="F48" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G47" s="11" t="s">
+      <c r="G48" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H47" s="11" t="s">
+      <c r="H48" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="I47" s="11" t="s">
+      <c r="I48" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="J47" s="11" t="s">
+      <c r="J48" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="K47" s="11" t="s">
+      <c r="K48" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="L47" s="11" t="s">
+      <c r="L48" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="M47" s="11" t="s">
+      <c r="M48" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="N47" s="11" t="s">
+      <c r="N48" s="11" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16">
-      <c r="A48" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B48" s="6">
-        <v>3431.6</v>
-      </c>
-      <c r="C48" s="6">
-        <v>10296.15</v>
-      </c>
-      <c r="D48" s="6">
-        <v>9311.3</v>
-      </c>
-      <c r="E48" s="6">
-        <v>4370.29</v>
-      </c>
-      <c r="F48" s="6">
-        <v>4507.02</v>
-      </c>
-      <c r="G48" s="6">
-        <v>11402.97</v>
-      </c>
-      <c r="H48" s="6"/>
-      <c r="I48" s="6"/>
-      <c r="J48" s="6"/>
-      <c r="K48" s="6"/>
-      <c r="L48" s="6"/>
-      <c r="M48" s="6"/>
-      <c r="N48" s="8">
-        <v>43319.33</v>
       </c>
     </row>
     <row r="49" spans="1:16">
       <c r="A49" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B49" s="6"/>
+        <v>31</v>
+      </c>
+      <c r="B49" s="6">
+        <v>3431.6</v>
+      </c>
       <c r="C49" s="6">
-        <v>448.0</v>
-      </c>
-      <c r="D49" s="6"/>
+        <v>10296.15</v>
+      </c>
+      <c r="D49" s="6">
+        <v>9311.3</v>
+      </c>
       <c r="E49" s="6">
-        <v>560.0</v>
+        <v>4370.29</v>
       </c>
       <c r="F49" s="6">
-        <v>840.0</v>
-      </c>
-      <c r="G49" s="6"/>
-      <c r="H49" s="6"/>
-      <c r="I49" s="6"/>
+        <v>4507.02</v>
+      </c>
+      <c r="G49" s="6">
+        <v>11402.97</v>
+      </c>
+      <c r="H49" s="6">
+        <v>14952.65</v>
+      </c>
+      <c r="I49" s="6">
+        <v>239.74</v>
+      </c>
       <c r="J49" s="6"/>
       <c r="K49" s="6"/>
       <c r="L49" s="6"/>
       <c r="M49" s="6"/>
       <c r="N49" s="8">
-        <v>1848.0</v>
+        <v>58511.72</v>
       </c>
     </row>
     <row r="50" spans="1:16">
       <c r="A50" s="4" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="B50" s="6"/>
       <c r="C50" s="6">
-        <v>210.0</v>
+        <v>448.0</v>
       </c>
       <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="6"/>
+      <c r="E50" s="6">
+        <v>560.0</v>
+      </c>
+      <c r="F50" s="6">
+        <v>840.0</v>
+      </c>
       <c r="G50" s="6"/>
       <c r="H50" s="6"/>
       <c r="I50" s="6"/>
@@ -2032,39 +2071,29 @@
       <c r="L50" s="6"/>
       <c r="M50" s="6"/>
       <c r="N50" s="8">
+        <v>1848.0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16">
+      <c r="A51" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B51" s="6"/>
+      <c r="C51" s="6">
         <v>210.0</v>
       </c>
-    </row>
-    <row r="51" spans="1:16">
-      <c r="A51" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B51" s="7">
-        <v>3431.6</v>
-      </c>
-      <c r="C51" s="7">
-        <v>10954.15</v>
-      </c>
-      <c r="D51" s="7">
-        <v>9311.3</v>
-      </c>
-      <c r="E51" s="7">
-        <v>4930.29</v>
-      </c>
-      <c r="F51" s="7">
-        <v>5347.02</v>
-      </c>
-      <c r="G51" s="7">
-        <v>11402.97</v>
-      </c>
-      <c r="H51" s="7"/>
-      <c r="I51" s="7"/>
-      <c r="J51" s="7"/>
-      <c r="K51" s="7"/>
-      <c r="L51" s="7"/>
-      <c r="M51" s="7"/>
-      <c r="N51" s="9">
-        <v>45377.33</v>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="6"/>
+      <c r="J51" s="6"/>
+      <c r="K51" s="6"/>
+      <c r="L51" s="6"/>
+      <c r="M51" s="6"/>
+      <c r="N51" s="8">
+        <v>210.0</v>
       </c>
     </row>
     <row r="52" spans="1:16">
@@ -2072,183 +2101,197 @@
         <v>26</v>
       </c>
       <c r="B52" s="7">
-        <f>IFERROR(AVERAGE(B48:B50),"")</f>
         <v>3431.6</v>
       </c>
       <c r="C52" s="7">
-        <f>IFERROR(AVERAGE(C48:C50),"")</f>
+        <v>10954.15</v>
+      </c>
+      <c r="D52" s="7">
+        <v>9311.3</v>
+      </c>
+      <c r="E52" s="7">
+        <v>4930.29</v>
+      </c>
+      <c r="F52" s="7">
+        <v>5347.02</v>
+      </c>
+      <c r="G52" s="7">
+        <v>11402.97</v>
+      </c>
+      <c r="H52" s="7">
+        <v>14952.65</v>
+      </c>
+      <c r="I52" s="7">
+        <v>239.74</v>
+      </c>
+      <c r="J52" s="7"/>
+      <c r="K52" s="7"/>
+      <c r="L52" s="7"/>
+      <c r="M52" s="7"/>
+      <c r="N52" s="9">
+        <v>60569.72</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16">
+      <c r="A53" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B53" s="7">
+        <f>IFERROR(AVERAGE(B49:B51),"")</f>
+        <v>3431.6</v>
+      </c>
+      <c r="C53" s="7">
+        <f>IFERROR(AVERAGE(C49:C51),"")</f>
         <v>3651.3833333333</v>
       </c>
-      <c r="D52" s="7">
-        <f>IFERROR(AVERAGE(D48:D50),"")</f>
+      <c r="D53" s="7">
+        <f>IFERROR(AVERAGE(D49:D51),"")</f>
         <v>9311.3</v>
       </c>
-      <c r="E52" s="7">
-        <f>IFERROR(AVERAGE(E48:E50),"")</f>
+      <c r="E53" s="7">
+        <f>IFERROR(AVERAGE(E49:E51),"")</f>
         <v>2465.145</v>
       </c>
-      <c r="F52" s="7">
-        <f>IFERROR(AVERAGE(F48:F50),"")</f>
+      <c r="F53" s="7">
+        <f>IFERROR(AVERAGE(F49:F51),"")</f>
         <v>2673.51</v>
       </c>
-      <c r="G52" s="7">
-        <f>IFERROR(AVERAGE(G48:G50),"")</f>
+      <c r="G53" s="7">
+        <f>IFERROR(AVERAGE(G49:G51),"")</f>
         <v>11402.97</v>
       </c>
-      <c r="H52" s="7" t="str">
-        <f>IFERROR(AVERAGE(H48:H50),"")</f>
+      <c r="H53" s="7">
+        <f>IFERROR(AVERAGE(H49:H51),"")</f>
+        <v>14952.65</v>
+      </c>
+      <c r="I53" s="7">
+        <f>IFERROR(AVERAGE(I49:I51),"")</f>
+        <v>239.74</v>
+      </c>
+      <c r="J53" s="7" t="str">
+        <f>IFERROR(AVERAGE(J49:J51),"")</f>
         <v/>
       </c>
-      <c r="I52" s="7" t="str">
-        <f>IFERROR(AVERAGE(I48:I50),"")</f>
+      <c r="K53" s="7" t="str">
+        <f>IFERROR(AVERAGE(K49:K51),"")</f>
         <v/>
       </c>
-      <c r="J52" s="7" t="str">
-        <f>IFERROR(AVERAGE(J48:J50),"")</f>
+      <c r="L53" s="7" t="str">
+        <f>IFERROR(AVERAGE(L49:L51),"")</f>
         <v/>
       </c>
-      <c r="K52" s="7" t="str">
-        <f>IFERROR(AVERAGE(K48:K50),"")</f>
+      <c r="M53" s="7" t="str">
+        <f>IFERROR(AVERAGE(M49:M51),"")</f>
         <v/>
       </c>
-      <c r="L52" s="7" t="str">
-        <f>IFERROR(AVERAGE(L48:L50),"")</f>
-        <v/>
-      </c>
-      <c r="M52" s="7" t="str">
-        <f>IFERROR(AVERAGE(M48:M50),"")</f>
-        <v/>
-      </c>
-      <c r="N52" s="9">
-        <f>IFERROR(AVERAGE(N48:N50),"")</f>
-        <v>15125.776666667</v>
-      </c>
-    </row>
-    <row r="54" spans="1:16">
-      <c r="A54" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B54" s="4"/>
-      <c r="C54" s="4"/>
-      <c r="D54" s="4"/>
-      <c r="E54" s="4"/>
-      <c r="F54" s="4"/>
-      <c r="G54" s="4"/>
-      <c r="H54" s="4"/>
-      <c r="I54" s="4"/>
-      <c r="J54" s="4"/>
-      <c r="K54" s="4"/>
-      <c r="L54" s="4"/>
-      <c r="M54" s="4"/>
-      <c r="N54" s="4"/>
+      <c r="N53" s="9">
+        <f>IFERROR(AVERAGE(N49:N51),"")</f>
+        <v>20189.906666667</v>
+      </c>
     </row>
     <row r="55" spans="1:16">
-      <c r="A55" s="11" t="s">
+      <c r="A55" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="4"/>
+      <c r="J55" s="4"/>
+      <c r="K55" s="4"/>
+      <c r="L55" s="4"/>
+      <c r="M55" s="4"/>
+      <c r="N55" s="4"/>
+    </row>
+    <row r="56" spans="1:16">
+      <c r="A56" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B55" s="11" t="s">
+      <c r="B56" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C55" s="11" t="s">
+      <c r="C56" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D55" s="11" t="s">
+      <c r="D56" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E55" s="11" t="s">
+      <c r="E56" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="F55" s="11" t="s">
+      <c r="F56" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="G55" s="11" t="s">
+      <c r="G56" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H55" s="11" t="s">
+      <c r="H56" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="I55" s="11" t="s">
+      <c r="I56" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="J55" s="11" t="s">
+      <c r="J56" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="K55" s="11" t="s">
+      <c r="K56" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="L55" s="11" t="s">
+      <c r="L56" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="M55" s="11" t="s">
+      <c r="M56" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="N55" s="11" t="s">
+      <c r="N56" s="11" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="56" spans="1:16">
-      <c r="A56" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B56" s="6">
-        <v>2862.0</v>
-      </c>
-      <c r="C56" s="6">
-        <v>9699.91</v>
-      </c>
-      <c r="D56" s="6">
-        <v>6628.18</v>
-      </c>
-      <c r="E56" s="6">
-        <v>1370.0</v>
-      </c>
-      <c r="F56" s="6">
-        <v>5727.92</v>
-      </c>
-      <c r="G56" s="6">
-        <v>6409.58</v>
-      </c>
-      <c r="H56" s="6">
-        <v>342.61</v>
-      </c>
-      <c r="I56" s="6"/>
-      <c r="J56" s="6"/>
-      <c r="K56" s="6"/>
-      <c r="L56" s="6"/>
-      <c r="M56" s="6"/>
-      <c r="N56" s="8">
-        <v>33040.2</v>
       </c>
     </row>
     <row r="57" spans="1:16">
       <c r="A57" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B57" s="6"/>
+        <v>31</v>
+      </c>
+      <c r="B57" s="6">
+        <v>2862.0</v>
+      </c>
       <c r="C57" s="6">
-        <v>448.0</v>
-      </c>
-      <c r="D57" s="6"/>
-      <c r="E57" s="6"/>
-      <c r="F57" s="6"/>
-      <c r="G57" s="6"/>
-      <c r="H57" s="6"/>
+        <v>9699.91</v>
+      </c>
+      <c r="D57" s="6">
+        <v>6628.18</v>
+      </c>
+      <c r="E57" s="6">
+        <v>1370.0</v>
+      </c>
+      <c r="F57" s="6">
+        <v>5727.92</v>
+      </c>
+      <c r="G57" s="6">
+        <v>6409.58</v>
+      </c>
+      <c r="H57" s="6">
+        <v>3699.28</v>
+      </c>
       <c r="I57" s="6"/>
       <c r="J57" s="6"/>
       <c r="K57" s="6"/>
       <c r="L57" s="6"/>
       <c r="M57" s="6"/>
       <c r="N57" s="8">
-        <v>448.0</v>
+        <v>36396.87</v>
       </c>
     </row>
     <row r="58" spans="1:16">
       <c r="A58" s="4" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="B58" s="6"/>
       <c r="C58" s="6">
-        <v>210.0</v>
+        <v>448.0</v>
       </c>
       <c r="D58" s="6"/>
       <c r="E58" s="6"/>
@@ -2261,41 +2304,29 @@
       <c r="L58" s="6"/>
       <c r="M58" s="6"/>
       <c r="N58" s="8">
+        <v>448.0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16">
+      <c r="A59" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B59" s="6"/>
+      <c r="C59" s="6">
         <v>210.0</v>
       </c>
-    </row>
-    <row r="59" spans="1:16">
-      <c r="A59" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B59" s="7">
-        <v>2862.0</v>
-      </c>
-      <c r="C59" s="7">
-        <v>10357.91</v>
-      </c>
-      <c r="D59" s="7">
-        <v>6628.18</v>
-      </c>
-      <c r="E59" s="7">
-        <v>1370.0</v>
-      </c>
-      <c r="F59" s="7">
-        <v>5727.92</v>
-      </c>
-      <c r="G59" s="7">
-        <v>6409.58</v>
-      </c>
-      <c r="H59" s="7">
-        <v>342.61</v>
-      </c>
-      <c r="I59" s="7"/>
-      <c r="J59" s="7"/>
-      <c r="K59" s="7"/>
-      <c r="L59" s="7"/>
-      <c r="M59" s="7"/>
-      <c r="N59" s="9">
-        <v>33698.2</v>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="6"/>
+      <c r="H59" s="6"/>
+      <c r="I59" s="6"/>
+      <c r="J59" s="6"/>
+      <c r="K59" s="6"/>
+      <c r="L59" s="6"/>
+      <c r="M59" s="6"/>
+      <c r="N59" s="8">
+        <v>210.0</v>
       </c>
     </row>
     <row r="60" spans="1:16">
@@ -2303,82 +2334,116 @@
         <v>26</v>
       </c>
       <c r="B60" s="7">
-        <f>IFERROR(AVERAGE(B56:B58),"")</f>
+        <v>2862.0</v>
+      </c>
+      <c r="C60" s="7">
+        <v>10357.91</v>
+      </c>
+      <c r="D60" s="7">
+        <v>6628.18</v>
+      </c>
+      <c r="E60" s="7">
+        <v>1370.0</v>
+      </c>
+      <c r="F60" s="7">
+        <v>5727.92</v>
+      </c>
+      <c r="G60" s="7">
+        <v>6409.58</v>
+      </c>
+      <c r="H60" s="7">
+        <v>3699.28</v>
+      </c>
+      <c r="I60" s="7"/>
+      <c r="J60" s="7"/>
+      <c r="K60" s="7"/>
+      <c r="L60" s="7"/>
+      <c r="M60" s="7"/>
+      <c r="N60" s="9">
+        <v>37054.87</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16">
+      <c r="A61" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B61" s="7">
+        <f>IFERROR(AVERAGE(B57:B59),"")</f>
         <v>2862</v>
       </c>
-      <c r="C60" s="7">
-        <f>IFERROR(AVERAGE(C56:C58),"")</f>
+      <c r="C61" s="7">
+        <f>IFERROR(AVERAGE(C57:C59),"")</f>
         <v>3452.6366666667</v>
       </c>
-      <c r="D60" s="7">
-        <f>IFERROR(AVERAGE(D56:D58),"")</f>
+      <c r="D61" s="7">
+        <f>IFERROR(AVERAGE(D57:D59),"")</f>
         <v>6628.18</v>
       </c>
-      <c r="E60" s="7">
-        <f>IFERROR(AVERAGE(E56:E58),"")</f>
+      <c r="E61" s="7">
+        <f>IFERROR(AVERAGE(E57:E59),"")</f>
         <v>1370</v>
       </c>
-      <c r="F60" s="7">
-        <f>IFERROR(AVERAGE(F56:F58),"")</f>
+      <c r="F61" s="7">
+        <f>IFERROR(AVERAGE(F57:F59),"")</f>
         <v>5727.92</v>
       </c>
-      <c r="G60" s="7">
-        <f>IFERROR(AVERAGE(G56:G58),"")</f>
+      <c r="G61" s="7">
+        <f>IFERROR(AVERAGE(G57:G59),"")</f>
         <v>6409.58</v>
       </c>
-      <c r="H60" s="7">
-        <f>IFERROR(AVERAGE(H56:H58),"")</f>
-        <v>342.61</v>
-      </c>
-      <c r="I60" s="7" t="str">
-        <f>IFERROR(AVERAGE(I56:I58),"")</f>
+      <c r="H61" s="7">
+        <f>IFERROR(AVERAGE(H57:H59),"")</f>
+        <v>3699.28</v>
+      </c>
+      <c r="I61" s="7" t="str">
+        <f>IFERROR(AVERAGE(I57:I59),"")</f>
         <v/>
       </c>
-      <c r="J60" s="7" t="str">
-        <f>IFERROR(AVERAGE(J56:J58),"")</f>
+      <c r="J61" s="7" t="str">
+        <f>IFERROR(AVERAGE(J57:J59),"")</f>
         <v/>
       </c>
-      <c r="K60" s="7" t="str">
-        <f>IFERROR(AVERAGE(K56:K58),"")</f>
+      <c r="K61" s="7" t="str">
+        <f>IFERROR(AVERAGE(K57:K59),"")</f>
         <v/>
       </c>
-      <c r="L60" s="7" t="str">
-        <f>IFERROR(AVERAGE(L56:L58),"")</f>
+      <c r="L61" s="7" t="str">
+        <f>IFERROR(AVERAGE(L57:L59),"")</f>
         <v/>
       </c>
-      <c r="M60" s="7" t="str">
-        <f>IFERROR(AVERAGE(M56:M58),"")</f>
+      <c r="M61" s="7" t="str">
+        <f>IFERROR(AVERAGE(M57:M59),"")</f>
         <v/>
       </c>
-      <c r="N60" s="9">
-        <f>IFERROR(AVERAGE(N56:N58),"")</f>
-        <v>11232.733333333</v>
-      </c>
-    </row>
-    <row r="63" spans="1:16">
-      <c r="A63" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B63" s="13">
-        <v>286032.95</v>
+      <c r="N61" s="9">
+        <f>IFERROR(AVERAGE(N57:N59),"")</f>
+        <v>12351.623333333</v>
       </c>
     </row>
     <row r="64" spans="1:16">
-      <c r="A64" s="14" t="s">
+      <c r="A64" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B64" s="15">
-        <v>192835.11</v>
+      <c r="B64" s="13">
+        <v>353770.8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16">
+      <c r="A65" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B65" s="15">
+        <v>227733.37</v>
       </c>
     </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="A1:N1"/>
-    <mergeCell ref="A16:N16"/>
-    <mergeCell ref="A27:N27"/>
-    <mergeCell ref="A36:N36"/>
-    <mergeCell ref="A46:N46"/>
-    <mergeCell ref="A54:N54"/>
+    <mergeCell ref="A17:N17"/>
+    <mergeCell ref="A28:N28"/>
+    <mergeCell ref="A37:N37"/>
+    <mergeCell ref="A47:N47"/>
+    <mergeCell ref="A55:N55"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2447,7 +2512,7 @@
   <sheetData>
     <row r="1" spans="1:37">
       <c r="A1" s="10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="4"/>
@@ -2554,117 +2619,117 @@
     <row r="3" spans="1:37">
       <c r="A3" s="4"/>
       <c r="B3" s="16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C3" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="F3" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" s="16" t="s">
+      <c r="G3" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="I3" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="H3" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="I3" s="16" t="s">
+      <c r="J3" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="K3" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="L3" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="K3" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="L3" s="16" t="s">
+      <c r="M3" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="N3" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="M3" s="16" t="s">
+      <c r="O3" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="N3" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="O3" s="16" t="s">
+      <c r="P3" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q3" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="R3" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="Q3" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="R3" s="16" t="s">
+      <c r="S3" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="T3" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="S3" s="16" t="s">
+      <c r="U3" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="T3" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="U3" s="16" t="s">
+      <c r="V3" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="W3" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="V3" s="16" t="s">
+      <c r="X3" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="W3" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="X3" s="16" t="s">
+      <c r="Y3" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z3" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="Y3" s="16" t="s">
+      <c r="AA3" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="Z3" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA3" s="16" t="s">
+      <c r="AB3" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC3" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="AB3" s="16" t="s">
+      <c r="AD3" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="AC3" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="AD3" s="16" t="s">
+      <c r="AE3" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF3" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="AE3" s="16" t="s">
+      <c r="AG3" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="AF3" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="AG3" s="16" t="s">
+      <c r="AH3" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="AI3" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="AH3" s="16" t="s">
+      <c r="AJ3" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="AI3" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ3" s="16" t="s">
-        <v>39</v>
-      </c>
       <c r="AK3" s="16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:37">
       <c r="A4" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B4" s="16">
         <v>119.0</v>
@@ -2709,7 +2774,7 @@
     </row>
     <row r="5" spans="1:37">
       <c r="A5" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B5" s="16"/>
       <c r="C5" s="4"/>
@@ -2750,7 +2815,7 @@
     </row>
     <row r="6" spans="1:37">
       <c r="A6" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B6" s="16"/>
       <c r="C6" s="4"/>
@@ -2793,7 +2858,7 @@
     </row>
     <row r="7" spans="1:37">
       <c r="A7" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" s="16"/>
       <c r="C7" s="4"/>
@@ -2834,7 +2899,7 @@
     </row>
     <row r="8" spans="1:37">
       <c r="A8" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8" s="16"/>
       <c r="C8" s="4"/>
@@ -2877,7 +2942,7 @@
     </row>
     <row r="9" spans="1:37">
       <c r="A9" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B9" s="17">
         <v>119.0</v>
@@ -2922,7 +2987,7 @@
     </row>
     <row r="11" spans="1:37">
       <c r="A11" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B11" s="16"/>
       <c r="C11" s="4"/>
@@ -3029,117 +3094,117 @@
     <row r="13" spans="1:37">
       <c r="A13" s="4"/>
       <c r="B13" s="16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C13" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="F13" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F13" s="16" t="s">
+      <c r="G13" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="G13" s="16" t="s">
+      <c r="I13" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="H13" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="I13" s="16" t="s">
+      <c r="J13" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="K13" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J13" s="16" t="s">
+      <c r="L13" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="K13" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="L13" s="16" t="s">
+      <c r="M13" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="N13" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="M13" s="16" t="s">
+      <c r="O13" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="N13" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="O13" s="16" t="s">
+      <c r="P13" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q13" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="P13" s="16" t="s">
+      <c r="R13" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="Q13" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="R13" s="16" t="s">
+      <c r="S13" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="T13" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="S13" s="16" t="s">
+      <c r="U13" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="T13" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="U13" s="16" t="s">
+      <c r="V13" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="W13" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="V13" s="16" t="s">
+      <c r="X13" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="W13" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="X13" s="16" t="s">
+      <c r="Y13" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z13" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="Y13" s="16" t="s">
+      <c r="AA13" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="Z13" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA13" s="16" t="s">
+      <c r="AB13" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC13" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="AB13" s="16" t="s">
+      <c r="AD13" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="AC13" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="AD13" s="16" t="s">
+      <c r="AE13" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF13" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="AE13" s="16" t="s">
+      <c r="AG13" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="AF13" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="AG13" s="16" t="s">
+      <c r="AH13" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="AI13" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="AH13" s="16" t="s">
+      <c r="AJ13" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="AI13" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ13" s="16" t="s">
-        <v>39</v>
-      </c>
       <c r="AK13" s="16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:37">
       <c r="A14" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B14" s="16">
         <v>50.0</v>
@@ -3184,7 +3249,7 @@
     </row>
     <row r="15" spans="1:37">
       <c r="A15" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B15" s="16"/>
       <c r="C15" s="4"/>
@@ -3225,7 +3290,7 @@
     </row>
     <row r="16" spans="1:37">
       <c r="A16" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B16" s="16"/>
       <c r="C16" s="4"/>
@@ -3268,7 +3333,7 @@
     </row>
     <row r="17" spans="1:37">
       <c r="A17" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" s="16"/>
       <c r="C17" s="4"/>
@@ -3309,7 +3374,7 @@
     </row>
     <row r="18" spans="1:37">
       <c r="A18" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B18" s="16"/>
       <c r="C18" s="4"/>
@@ -3352,7 +3417,7 @@
     </row>
     <row r="19" spans="1:37">
       <c r="A19" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B19" s="17">
         <v>50.0</v>
@@ -3397,7 +3462,7 @@
     </row>
     <row r="21" spans="1:37">
       <c r="A21" s="10" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B21" s="16"/>
       <c r="C21" s="4"/>
@@ -3504,117 +3569,117 @@
     <row r="23" spans="1:37">
       <c r="A23" s="4"/>
       <c r="B23" s="16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C23" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="16" t="s">
+      <c r="F23" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E23" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F23" s="16" t="s">
+      <c r="G23" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="H23" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="G23" s="16" t="s">
+      <c r="I23" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="H23" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="I23" s="16" t="s">
+      <c r="J23" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="K23" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="J23" s="16" t="s">
+      <c r="L23" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="K23" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="L23" s="16" t="s">
+      <c r="M23" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="N23" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="M23" s="16" t="s">
+      <c r="O23" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="N23" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="O23" s="16" t="s">
+      <c r="P23" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q23" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="P23" s="16" t="s">
+      <c r="R23" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="Q23" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="R23" s="16" t="s">
+      <c r="S23" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="T23" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="S23" s="16" t="s">
+      <c r="U23" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="T23" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="U23" s="16" t="s">
+      <c r="V23" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="W23" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="V23" s="16" t="s">
+      <c r="X23" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="W23" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="X23" s="16" t="s">
+      <c r="Y23" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z23" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="Y23" s="16" t="s">
+      <c r="AA23" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="Z23" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA23" s="16" t="s">
+      <c r="AB23" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC23" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="AB23" s="16" t="s">
+      <c r="AD23" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="AC23" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="AD23" s="16" t="s">
+      <c r="AE23" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF23" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="AE23" s="16" t="s">
+      <c r="AG23" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="AF23" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="AG23" s="16" t="s">
+      <c r="AH23" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="AI23" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="AH23" s="16" t="s">
+      <c r="AJ23" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="AI23" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="AJ23" s="16" t="s">
-        <v>39</v>
-      </c>
       <c r="AK23" s="16" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:37">
       <c r="A24" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B24" s="16">
         <v>40.0</v>
@@ -3659,7 +3724,7 @@
     </row>
     <row r="25" spans="1:37">
       <c r="A25" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B25" s="16"/>
       <c r="C25" s="4"/>
@@ -3700,7 +3765,7 @@
     </row>
     <row r="26" spans="1:37">
       <c r="A26" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B26" s="16"/>
       <c r="C26" s="4"/>
@@ -3743,7 +3808,7 @@
     </row>
     <row r="27" spans="1:37">
       <c r="A27" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B27" s="16"/>
       <c r="C27" s="4"/>
@@ -3784,7 +3849,7 @@
     </row>
     <row r="28" spans="1:37">
       <c r="A28" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B28" s="16"/>
       <c r="C28" s="4"/>
@@ -3827,7 +3892,7 @@
     </row>
     <row r="29" spans="1:37">
       <c r="A29" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B29" s="17">
         <v>40.0</v>

</xml_diff>